<commit_message>
updates to contacts/pt (in 24hr period)
</commit_message>
<xml_diff>
--- a/PPE_calculator.xlsx
+++ b/PPE_calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eotles/Documents/workspace/covid_staffing_exo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9B3286-7AB0-4643-95F2-B0BE39B892CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CC3204-9D4C-E647-A0CF-133D9AABFBBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36600" yWindow="-8540" windowWidth="41780" windowHeight="26400" xr2:uid="{CE7FBBC9-ED7D-2B46-9B81-72B960D0E09A}"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20540" xr2:uid="{CE7FBBC9-ED7D-2B46-9B81-72B960D0E09A}"/>
   </bookViews>
   <sheets>
     <sheet name="roll-up" sheetId="1" r:id="rId1"/>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>your inputs</t>
-  </si>
-  <si>
-    <t>Contacts / Pt</t>
   </si>
   <si>
     <t>Items Used / Contact</t>
@@ -305,6 +302,9 @@
   </si>
   <si>
     <t>ICU</t>
+  </si>
+  <si>
+    <t>Contacts / Pt (in 24hr period)</t>
   </si>
 </sst>
 </file>
@@ -1091,48 +1091,6 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1156,9 +1114,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1175,6 +1130,51 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2002,7 +2002,7 @@
   <dimension ref="A1:AW37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -2029,43 +2029,43 @@
   <sheetData>
     <row r="1" spans="2:48" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:48" x14ac:dyDescent="0.2">
-      <c r="B2" s="81"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
-      <c r="L2" s="82"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
     </row>
     <row r="3" spans="2:48" x14ac:dyDescent="0.2">
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
     </row>
     <row r="4" spans="2:48" x14ac:dyDescent="0.2">
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="82"/>
+      <c r="B4" s="97"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="97"/>
     </row>
     <row r="5" spans="2:48" x14ac:dyDescent="0.2">
       <c r="B5" s="66"/>
@@ -2095,36 +2095,36 @@
     </row>
     <row r="7" spans="2:48" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:48" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="88"/>
+      <c r="B8" s="74"/>
       <c r="C8" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="72" t="s">
+      <c r="E8" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="72" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="72" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="72" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="72" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="K8" s="72" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" s="73" t="s">
         <v>51</v>
-      </c>
-      <c r="E8" s="72" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="72" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="72" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="72" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="72" t="s">
-        <v>47</v>
-      </c>
-      <c r="J8" s="72" t="s">
-        <v>48</v>
-      </c>
-      <c r="K8" s="72" t="s">
-        <v>49</v>
-      </c>
-      <c r="L8" s="73" t="s">
-        <v>52</v>
       </c>
       <c r="N8" s="9" t="s">
         <v>24</v>
@@ -2356,52 +2356,52 @@
       <c r="AV12" s="32"/>
     </row>
     <row r="13" spans="2:48" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="89"/>
-      <c r="C13" s="74" t="s">
+      <c r="B13" s="75"/>
+      <c r="C13" s="88" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="88"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="88"/>
+      <c r="G13" s="88"/>
+      <c r="H13" s="88"/>
+      <c r="I13" s="88"/>
+      <c r="J13" s="88"/>
+      <c r="K13" s="88"/>
+      <c r="L13" s="89"/>
+      <c r="N13" s="74"/>
+      <c r="O13" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="74"/>
-      <c r="J13" s="74"/>
-      <c r="K13" s="74"/>
-      <c r="L13" s="75"/>
-      <c r="N13" s="88"/>
-      <c r="O13" s="96" t="s">
-        <v>26</v>
-      </c>
-      <c r="P13" s="76"/>
-      <c r="Q13" s="76"/>
-      <c r="R13" s="76"/>
-      <c r="S13" s="76"/>
-      <c r="T13" s="76"/>
-      <c r="U13" s="76"/>
-      <c r="V13" s="76"/>
-      <c r="W13" s="76"/>
-      <c r="X13" s="77"/>
-      <c r="Y13" s="94" t="s">
+      <c r="P13" s="91"/>
+      <c r="Q13" s="91"/>
+      <c r="R13" s="91"/>
+      <c r="S13" s="91"/>
+      <c r="T13" s="91"/>
+      <c r="U13" s="91"/>
+      <c r="V13" s="91"/>
+      <c r="W13" s="91"/>
+      <c r="X13" s="92"/>
+      <c r="Y13" s="80" t="s">
         <v>15</v>
       </c>
       <c r="Z13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AK13" s="90"/>
-      <c r="AL13" s="78" t="s">
+      <c r="AK13" s="76"/>
+      <c r="AL13" s="93" t="s">
         <v>22</v>
       </c>
-      <c r="AM13" s="79"/>
-      <c r="AN13" s="79"/>
-      <c r="AO13" s="79"/>
-      <c r="AP13" s="79"/>
-      <c r="AQ13" s="79"/>
-      <c r="AR13" s="79"/>
-      <c r="AS13" s="79"/>
-      <c r="AT13" s="79"/>
-      <c r="AU13" s="79"/>
-      <c r="AV13" s="80"/>
+      <c r="AM13" s="94"/>
+      <c r="AN13" s="94"/>
+      <c r="AO13" s="94"/>
+      <c r="AP13" s="94"/>
+      <c r="AQ13" s="94"/>
+      <c r="AR13" s="94"/>
+      <c r="AS13" s="94"/>
+      <c r="AT13" s="94"/>
+      <c r="AU13" s="94"/>
+      <c r="AV13" s="95"/>
     </row>
     <row r="14" spans="2:48" ht="30" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="44" t="s">
@@ -2486,7 +2486,7 @@
         <f t="shared" si="1"/>
         <v>COVID Consult</v>
       </c>
-      <c r="X14" s="95" t="str">
+      <c r="X14" s="81" t="str">
         <f>L8</f>
         <v>ICU</v>
       </c>
@@ -2537,43 +2537,43 @@
         <f>N14</f>
         <v>Item</v>
       </c>
-      <c r="AL14" s="91" t="str">
+      <c r="AL14" s="77" t="str">
         <f>C8</f>
         <v>Floor</v>
       </c>
-      <c r="AM14" s="92" t="str">
+      <c r="AM14" s="78" t="str">
         <f>D8</f>
         <v>Step-down</v>
       </c>
-      <c r="AN14" s="92" t="str">
+      <c r="AN14" s="78" t="str">
         <f t="shared" ref="AN14:AT14" si="3">E8</f>
         <v>COVID floor</v>
       </c>
-      <c r="AO14" s="92" t="str">
+      <c r="AO14" s="78" t="str">
         <f t="shared" si="3"/>
         <v>COVID ICU Step-Down</v>
       </c>
-      <c r="AP14" s="92" t="str">
+      <c r="AP14" s="78" t="str">
         <f t="shared" si="3"/>
         <v>COVID ICU Intubated</v>
       </c>
-      <c r="AQ14" s="92" t="str">
+      <c r="AQ14" s="78" t="str">
         <f t="shared" si="3"/>
         <v>Non-COVID floor</v>
       </c>
-      <c r="AR14" s="92" t="str">
+      <c r="AR14" s="78" t="str">
         <f t="shared" si="3"/>
         <v>Non-COVID SD</v>
       </c>
-      <c r="AS14" s="92" t="str">
+      <c r="AS14" s="78" t="str">
         <f t="shared" si="3"/>
         <v>Non-COVID ICU</v>
       </c>
-      <c r="AT14" s="92" t="str">
+      <c r="AT14" s="78" t="str">
         <f t="shared" si="3"/>
         <v>COVID Consult</v>
       </c>
-      <c r="AU14" s="93" t="str">
+      <c r="AU14" s="79" t="str">
         <f>L8</f>
         <v>ICU</v>
       </c>
@@ -2681,51 +2681,51 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AK15" s="98" t="str">
+      <c r="AK15" s="83" t="str">
         <f t="shared" ref="AK15:AK35" si="5">IF(ISBLANK(N15),"",N15)</f>
         <v>N95 Mask</v>
       </c>
-      <c r="AL15" s="99">
+      <c r="AL15" s="84">
         <f t="shared" ref="AL15:AM21" si="6">IFERROR(ROUNDUP(C$9*C$36*Z15,0), "")</f>
         <v>0</v>
       </c>
-      <c r="AM15" s="100">
+      <c r="AM15" s="85">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AN15" s="100">
+      <c r="AN15" s="85">
         <f t="shared" ref="AN15:AT21" si="7">IFERROR(ROUNDUP(E$9*E$36*AB15,0), "")</f>
         <v>0</v>
       </c>
-      <c r="AO15" s="100">
+      <c r="AO15" s="85">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AP15" s="100">
+      <c r="AP15" s="85">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AQ15" s="100">
+      <c r="AQ15" s="85">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AR15" s="100">
+      <c r="AR15" s="85">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AS15" s="100">
+      <c r="AS15" s="85">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AT15" s="100">
+      <c r="AT15" s="85">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AU15" s="101">
+      <c r="AU15" s="86">
         <f t="shared" ref="AU15:AU35" si="8">IFERROR(ROUNDUP(L$9*L$36*AI15,0),"")</f>
         <v>0</v>
       </c>
-      <c r="AV15" s="102">
+      <c r="AV15" s="87">
         <f>IFERROR(SUM(AL15:AU15),"")</f>
         <v>0</v>
       </c>
@@ -2885,7 +2885,7 @@
     </row>
     <row r="17" spans="2:48" x14ac:dyDescent="0.2">
       <c r="B17" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="47">
         <v>8</v>
@@ -3024,7 +3024,7 @@
     </row>
     <row r="18" spans="2:48" x14ac:dyDescent="0.2">
       <c r="B18" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" s="47">
         <v>2</v>
@@ -3470,7 +3470,7 @@
       <c r="K21" s="47"/>
       <c r="L21" s="13"/>
       <c r="N21" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O21" s="5">
         <v>0</v>
@@ -3607,7 +3607,7 @@
         <v>2</v>
       </c>
       <c r="N22" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O22" s="5">
         <v>1</v>
@@ -3900,7 +3900,7 @@
     </row>
     <row r="26" spans="2:48" x14ac:dyDescent="0.2">
       <c r="B26" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="47">
         <v>0.5</v>
@@ -3985,7 +3985,7 @@
     </row>
     <row r="27" spans="2:48" x14ac:dyDescent="0.2">
       <c r="B27" s="67" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" s="47">
         <v>1</v>
@@ -4070,7 +4070,7 @@
     </row>
     <row r="28" spans="2:48" x14ac:dyDescent="0.2">
       <c r="B28" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="47"/>
@@ -4585,7 +4585,7 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AV35" s="97">
+      <c r="AV35" s="82">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -4799,17 +4799,17 @@
     </row>
     <row r="13" spans="2:12" ht="71" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="38"/>
-      <c r="C13" s="87" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="87"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="87"/>
-      <c r="J13" s="87"/>
-      <c r="K13" s="87"/>
+      <c r="C13" s="102" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="102"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="102"/>
+      <c r="G13" s="102"/>
+      <c r="H13" s="102"/>
+      <c r="I13" s="102"/>
+      <c r="J13" s="102"/>
+      <c r="K13" s="102"/>
       <c r="L13" s="36"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
@@ -4829,7 +4829,7 @@
       <c r="B15" s="38"/>
       <c r="C15" s="37"/>
       <c r="D15" s="40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" s="39"/>
       <c r="F15" s="39"/>
@@ -4844,7 +4844,7 @@
       <c r="B16" s="38"/>
       <c r="C16" s="37"/>
       <c r="D16" s="40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" s="39"/>
       <c r="F16" s="39"/>
@@ -4859,7 +4859,7 @@
       <c r="B17" s="38"/>
       <c r="C17" s="37"/>
       <c r="D17" s="40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E17" s="39"/>
       <c r="F17" s="39"/>
@@ -4885,17 +4885,17 @@
     </row>
     <row r="19" spans="2:12" ht="81" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="38"/>
-      <c r="C19" s="87" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="87"/>
-      <c r="E19" s="87"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="87"/>
-      <c r="H19" s="87"/>
-      <c r="I19" s="87"/>
-      <c r="J19" s="87"/>
-      <c r="K19" s="87"/>
+      <c r="C19" s="102" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="102"/>
+      <c r="E19" s="102"/>
+      <c r="F19" s="102"/>
+      <c r="G19" s="102"/>
+      <c r="H19" s="102"/>
+      <c r="I19" s="102"/>
+      <c r="J19" s="102"/>
+      <c r="K19" s="102"/>
       <c r="L19" s="36"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
@@ -4913,17 +4913,17 @@
     </row>
     <row r="21" spans="2:12" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="38"/>
-      <c r="C21" s="87" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="87"/>
-      <c r="E21" s="87"/>
-      <c r="F21" s="87"/>
-      <c r="G21" s="87"/>
-      <c r="H21" s="87"/>
-      <c r="I21" s="87"/>
-      <c r="J21" s="87"/>
-      <c r="K21" s="87"/>
+      <c r="C21" s="102" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="102"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="102"/>
+      <c r="G21" s="102"/>
+      <c r="H21" s="102"/>
+      <c r="I21" s="102"/>
+      <c r="J21" s="102"/>
+      <c r="K21" s="102"/>
       <c r="L21" s="36"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
@@ -4941,17 +4941,17 @@
     </row>
     <row r="23" spans="2:12" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="38"/>
-      <c r="C23" s="87" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="87"/>
-      <c r="H23" s="87"/>
-      <c r="I23" s="87"/>
-      <c r="J23" s="87"/>
-      <c r="K23" s="87"/>
+      <c r="C23" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="102"/>
+      <c r="E23" s="102"/>
+      <c r="F23" s="102"/>
+      <c r="G23" s="102"/>
+      <c r="H23" s="102"/>
+      <c r="I23" s="102"/>
+      <c r="J23" s="102"/>
+      <c r="K23" s="102"/>
       <c r="L23" s="36"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.2">
@@ -4970,14 +4970,14 @@
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" s="38"/>
       <c r="C25" s="37"/>
-      <c r="D25" s="86" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="86"/>
-      <c r="H25" s="86"/>
-      <c r="I25" s="86"/>
+      <c r="D25" s="101" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="101"/>
+      <c r="F25" s="101"/>
+      <c r="G25" s="101"/>
+      <c r="H25" s="101"/>
+      <c r="I25" s="101"/>
       <c r="J25" s="37"/>
       <c r="K25" s="37"/>
       <c r="L25" s="36"/>
@@ -4996,19 +4996,19 @@
       <c r="L26" s="33"/>
     </row>
     <row r="27" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="83" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="84"/>
-      <c r="D27" s="84"/>
-      <c r="E27" s="84"/>
-      <c r="F27" s="84"/>
-      <c r="G27" s="84"/>
-      <c r="H27" s="84"/>
-      <c r="I27" s="84"/>
-      <c r="J27" s="84"/>
-      <c r="K27" s="84"/>
-      <c r="L27" s="85"/>
+      <c r="B27" s="98" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="99"/>
+      <c r="D27" s="99"/>
+      <c r="E27" s="99"/>
+      <c r="F27" s="99"/>
+      <c r="G27" s="99"/>
+      <c r="H27" s="99"/>
+      <c r="I27" s="99"/>
+      <c r="J27" s="99"/>
+      <c r="K27" s="99"/>
+      <c r="L27" s="100"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>

</xml_diff>